<commit_message>
Dan commit to catchup
</commit_message>
<xml_diff>
--- a/Document Table.xlsx
+++ b/Document Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfreeman\Documents\ModelCatalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dashney\Documents\Clones\ModelCatalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{209DD14B-E089-405B-9456-DBBDFD0538BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6917BAC7-8B84-4ED8-AA8A-6EB50B421475}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{7BD1DB24-80EA-454E-A892-E0C055D34D67}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
-  <si>
-    <t>Capabilities</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Working</t>
   </si>
@@ -60,32 +57,62 @@
     <t>Prompts for and Accepts, Model Alterations File when Model Alterations are selected</t>
   </si>
   <si>
-    <t>Calibrates Model using parameters pin provided Excel file path</t>
-  </si>
-  <si>
     <t>Prompts for Model Status of Working or Final</t>
   </si>
   <si>
-    <t>Model is Altered using provided Alterations file</t>
-  </si>
-  <si>
     <t>Accepts Project Phases of: Planning, Pre-Design, 30, 60, and 90 percent</t>
   </si>
   <si>
-    <t>Working Models are registered in Model Catalog</t>
-  </si>
-  <si>
     <t>Final Models are registered in RRAD</t>
   </si>
   <si>
-    <t>RRAD Subsets Stroms</t>
+    <t>RRAD Subsets Storms</t>
+  </si>
+  <si>
+    <t>All Models are registered in Model Catalog</t>
+  </si>
+  <si>
+    <t>Model Capabilities</t>
+  </si>
+  <si>
+    <t>Rehab Capabilities</t>
+  </si>
+  <si>
+    <t>Calculates APW</t>
+  </si>
+  <si>
+    <t>Calculates Capital Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate risk in dollars </t>
+  </si>
+  <si>
+    <t>Read Rehab.nBCR_data and Rehab.Branches</t>
+  </si>
+  <si>
+    <t>Generate Rehab ID</t>
+  </si>
+  <si>
+    <t>Attach information from Branches to nBCR_data</t>
+  </si>
+  <si>
+    <t>Delete unnecessary fields</t>
+  </si>
+  <si>
+    <t>Attach geometry to tabular information</t>
+  </si>
+  <si>
+    <t>Append pipes to RRAD</t>
+  </si>
+  <si>
+    <t>Generalized geometry created for model area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +120,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -169,28 +209,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -212,34 +230,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -259,36 +280,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -600,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F27845A-8D4B-40FE-815D-F493AE3920E8}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A2:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,153 +638,143 @@
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>9</v>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="13"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -771,54 +786,92 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,13 +882,15 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -848,6 +903,9 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Dan commit to catchup"
This reverts commit a2ffbfe8e8e1de83e158afb1e91dff7ae5478fd9.
</commit_message>
<xml_diff>
--- a/Document Table.xlsx
+++ b/Document Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dashney\Documents\Clones\ModelCatalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfreeman\Documents\ModelCatalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6917BAC7-8B84-4ED8-AA8A-6EB50B421475}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{209DD14B-E089-405B-9456-DBBDFD0538BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{7BD1DB24-80EA-454E-A892-E0C055D34D67}"/>
   </bookViews>
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+  <si>
+    <t>Capabilities</t>
+  </si>
   <si>
     <t>Working</t>
   </si>
@@ -57,62 +60,32 @@
     <t>Prompts for and Accepts, Model Alterations File when Model Alterations are selected</t>
   </si>
   <si>
+    <t>Calibrates Model using parameters pin provided Excel file path</t>
+  </si>
+  <si>
     <t>Prompts for Model Status of Working or Final</t>
   </si>
   <si>
+    <t>Model is Altered using provided Alterations file</t>
+  </si>
+  <si>
     <t>Accepts Project Phases of: Planning, Pre-Design, 30, 60, and 90 percent</t>
   </si>
   <si>
+    <t>Working Models are registered in Model Catalog</t>
+  </si>
+  <si>
     <t>Final Models are registered in RRAD</t>
   </si>
   <si>
-    <t>RRAD Subsets Storms</t>
-  </si>
-  <si>
-    <t>All Models are registered in Model Catalog</t>
-  </si>
-  <si>
-    <t>Model Capabilities</t>
-  </si>
-  <si>
-    <t>Rehab Capabilities</t>
-  </si>
-  <si>
-    <t>Calculates APW</t>
-  </si>
-  <si>
-    <t>Calculates Capital Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculate risk in dollars </t>
-  </si>
-  <si>
-    <t>Read Rehab.nBCR_data and Rehab.Branches</t>
-  </si>
-  <si>
-    <t>Generate Rehab ID</t>
-  </si>
-  <si>
-    <t>Attach information from Branches to nBCR_data</t>
-  </si>
-  <si>
-    <t>Delete unnecessary fields</t>
-  </si>
-  <si>
-    <t>Attach geometry to tabular information</t>
-  </si>
-  <si>
-    <t>Append pipes to RRAD</t>
-  </si>
-  <si>
-    <t>Generalized geometry created for model area</t>
+    <t>RRAD Subsets Stroms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,29 +93,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -209,6 +169,28 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -230,6 +212,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -240,27 +235,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -280,40 +259,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -625,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F27845A-8D4B-40FE-815D-F493AE3920E8}">
-  <dimension ref="A2:C39"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,143 +613,153 @@
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="9" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>8</v>
-      </c>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>8</v>
-      </c>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="11"/>
+      <c r="A16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13"/>
       <c r="C16" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="14"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -786,92 +771,54 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>1</v>
-      </c>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,15 +829,13 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -903,9 +848,6 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>